<commit_message>
Data Transformation Done, Here I have used the dataset clean data set, which I have cleaned in the previous chapter
</commit_message>
<xml_diff>
--- a/real-estate.xlsx
+++ b/real-estate.xlsx
@@ -908,7 +908,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,8 +916,10 @@
     <col min="1" max="1" width="21.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="1" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="1"/>
+    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>